<commit_message>
résolution de problèmes et modification base d'une recette
</commit_message>
<xml_diff>
--- a/liste des ingrédients.xlsx
+++ b/liste des ingrédients.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bloew\Desktop\DEV\Projets-applications\FoodLove\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2781EE-4C47-4F10-A658-735BEA216AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F086DA-9BF9-4DA5-90DC-15D5BA9CDCB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="3450" windowWidth="19080" windowHeight="10035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="6740" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$106</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$105</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="168">
   <si>
     <t>Catégories</t>
   </si>
@@ -309,9 +309,6 @@
   </si>
   <si>
     <t>chair à saucisse</t>
-  </si>
-  <si>
-    <t>cote filet</t>
   </si>
   <si>
     <t>filet mignon</t>
@@ -1031,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G123"/>
+  <dimension ref="A1:G122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,40 +1049,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1096,7 +1093,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1107,7 +1104,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1118,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1129,7 +1126,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1140,7 +1137,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1151,7 +1148,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1162,7 +1159,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1173,7 +1170,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1184,7 +1181,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1195,7 +1192,7 @@
         <v>17</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1206,7 +1203,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1217,7 +1214,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1228,7 +1225,7 @@
         <v>20</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1239,7 +1236,7 @@
         <v>21</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1250,7 +1247,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1261,7 +1258,7 @@
         <v>23</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1272,7 +1269,7 @@
         <v>24</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1283,7 +1280,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1294,7 +1291,7 @@
         <v>26</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1305,7 +1302,7 @@
         <v>27</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1316,7 +1313,7 @@
         <v>28</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1327,7 +1324,7 @@
         <v>29</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1338,7 +1335,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1349,7 +1346,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1360,7 +1357,7 @@
         <v>32</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1371,7 +1368,7 @@
         <v>33</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1382,7 +1379,7 @@
         <v>34</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1393,7 +1390,7 @@
         <v>35</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1404,7 +1401,7 @@
         <v>36</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1415,7 +1412,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1426,7 +1423,7 @@
         <v>38</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1437,7 +1434,7 @@
         <v>39</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1448,7 +1445,7 @@
         <v>40</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1459,7 +1456,7 @@
         <v>41</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1470,7 +1467,7 @@
         <v>42</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1481,7 +1478,7 @@
         <v>43</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1492,7 +1489,7 @@
         <v>44</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1503,7 +1500,7 @@
         <v>45</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1514,7 +1511,7 @@
         <v>46</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1525,7 +1522,7 @@
         <v>47</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1536,7 +1533,7 @@
         <v>48</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1547,7 +1544,7 @@
         <v>49</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1558,7 +1555,7 @@
         <v>50</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1569,7 +1566,7 @@
         <v>51</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1580,7 +1577,7 @@
         <v>55</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1591,7 +1588,7 @@
         <v>56</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -1602,7 +1599,7 @@
         <v>57</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -1613,7 +1610,7 @@
         <v>58</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -1624,7 +1621,7 @@
         <v>60</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1635,7 +1632,7 @@
         <v>59</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -1646,7 +1643,7 @@
         <v>61</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G55" s="21"/>
     </row>
@@ -1658,7 +1655,7 @@
         <v>62</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -1669,7 +1666,7 @@
         <v>63</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -1680,7 +1677,7 @@
         <v>64</v>
       </c>
       <c r="C58" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -1691,7 +1688,7 @@
         <v>65</v>
       </c>
       <c r="C59" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -1702,7 +1699,7 @@
         <v>66</v>
       </c>
       <c r="C60" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -1713,7 +1710,7 @@
         <v>67</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -1724,7 +1721,7 @@
         <v>69</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -1735,7 +1732,7 @@
         <v>68</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -1746,7 +1743,7 @@
         <v>70</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1757,7 +1754,7 @@
         <v>71</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1768,7 +1765,7 @@
         <v>72</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1779,7 +1776,7 @@
         <v>73</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1790,7 +1787,7 @@
         <v>74</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1801,7 +1798,7 @@
         <v>75</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1812,7 +1809,7 @@
         <v>76</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1823,7 +1820,7 @@
         <v>77</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1834,7 +1831,7 @@
         <v>78</v>
       </c>
       <c r="C72" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1845,7 +1842,7 @@
         <v>79</v>
       </c>
       <c r="C73" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1856,7 +1853,7 @@
         <v>80</v>
       </c>
       <c r="C74" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1867,7 +1864,7 @@
         <v>81</v>
       </c>
       <c r="C75" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1878,7 +1875,7 @@
         <v>82</v>
       </c>
       <c r="C76" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1889,7 +1886,7 @@
         <v>83</v>
       </c>
       <c r="C77" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1900,7 +1897,7 @@
         <v>84</v>
       </c>
       <c r="C78" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1911,7 +1908,7 @@
         <v>85</v>
       </c>
       <c r="C79" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1922,7 +1919,7 @@
         <v>86</v>
       </c>
       <c r="C80" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1933,7 +1930,7 @@
         <v>87</v>
       </c>
       <c r="C81" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1944,7 +1941,7 @@
         <v>88</v>
       </c>
       <c r="C82" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1955,7 +1952,7 @@
         <v>89</v>
       </c>
       <c r="C83" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1966,7 +1963,7 @@
         <v>90</v>
       </c>
       <c r="C84" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1977,7 +1974,7 @@
         <v>91</v>
       </c>
       <c r="C85" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1988,7 +1985,7 @@
         <v>92</v>
       </c>
       <c r="C86" s="22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1999,7 +1996,7 @@
         <v>93</v>
       </c>
       <c r="C87" s="22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -2010,7 +2007,7 @@
         <v>94</v>
       </c>
       <c r="C88" s="22" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -2021,7 +2018,7 @@
         <v>95</v>
       </c>
       <c r="C89" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -2032,7 +2029,7 @@
         <v>96</v>
       </c>
       <c r="C90" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -2043,7 +2040,7 @@
         <v>97</v>
       </c>
       <c r="C91" s="22" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -2054,7 +2051,7 @@
         <v>98</v>
       </c>
       <c r="C92" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -2065,7 +2062,7 @@
         <v>99</v>
       </c>
       <c r="C93" s="22" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -2076,7 +2073,7 @@
         <v>100</v>
       </c>
       <c r="C94" s="22" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -2087,7 +2084,7 @@
         <v>101</v>
       </c>
       <c r="C95" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -2095,10 +2092,10 @@
         <v>7</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="C96" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -2106,10 +2103,10 @@
         <v>7</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="C97" s="22" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -2120,7 +2117,7 @@
         <v>103</v>
       </c>
       <c r="C98" s="22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -2131,7 +2128,7 @@
         <v>104</v>
       </c>
       <c r="C99" s="22" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -2142,7 +2139,7 @@
         <v>105</v>
       </c>
       <c r="C100" s="22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -2164,7 +2161,7 @@
         <v>107</v>
       </c>
       <c r="C102" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -2175,7 +2172,7 @@
         <v>108</v>
       </c>
       <c r="C103" s="22" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -2186,7 +2183,7 @@
         <v>109</v>
       </c>
       <c r="C104" s="22" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -2197,18 +2194,18 @@
         <v>110</v>
       </c>
       <c r="C105" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B106" s="11" t="s">
+      <c r="B106" s="12" t="s">
         <v>111</v>
       </c>
       <c r="C106" s="22" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -2219,19 +2216,12 @@
         <v>112</v>
       </c>
       <c r="C107" s="22" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B108" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C108" s="22" t="s">
-        <v>164</v>
-      </c>
+      <c r="A108" s="3"/>
+      <c r="B108" s="5"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
@@ -2289,14 +2279,10 @@
       <c r="A122" s="3"/>
       <c r="B122" s="5"/>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="3"/>
-      <c r="B123" s="5"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:B106" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B108">
-      <sortCondition ref="A1:A106"/>
+  <autoFilter ref="A1:B105" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B107">
+      <sortCondition ref="A1:A105"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>